<commit_message>
Added static JSON required for Kings test word docs
</commit_message>
<xml_diff>
--- a/docs/Kings-HelperFieldMappings.xlsx
+++ b/docs/Kings-HelperFieldMappings.xlsx
@@ -19,7 +19,9 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$44</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Example 4'!$A$2:$H$35</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -2494,10 +2496,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4249,6 +4251,7 @@
         <v>128</v>
       </c>
     </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>

</xml_diff>

<commit_message>
Added schema checks and templated schema checks for generated CDA document as part of unit test, and added missing keys in test JSON
</commit_message>
<xml_diff>
--- a/docs/Kings-HelperFieldMappings.xlsx
+++ b/docs/Kings-HelperFieldMappings.xlsx
@@ -20,8 +20,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Examples 2 and 3'!$A$2:$H$44</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Example 4'!$A$2:$H$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'Example 4'!$A$2:$H$35</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -2498,8 +2500,8 @@
   </sheetPr>
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>